<commit_message>
update user log, add replikasi vm, dll
</commit_message>
<xml_diff>
--- a/public/template_xls/template_aplikasi.xlsx
+++ b/public/template_xls/template_aplikasi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bankbtn-my.sharepoint.com/personal/ivan20057_btn_co_id/Documents/Documents/IES Portal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bankbtn-my.sharepoint.com/personal/ivan20057_btn_co_id/Documents/Documents/IES Portal/template_xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{E4EF04D0-9D9C-46D9-B554-F86F215F04D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E697B691-13AC-40E8-94D1-E66D6558B5C5}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{E4EF04D0-9D9C-46D9-B554-F86F215F04D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99364219-4D7B-418F-93B9-BB4935E8B7B1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F36BE757-7840-428F-B9FD-226C1B34BFAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Susilo</t>
   </si>
@@ -60,13 +60,41 @@
   </si>
   <si>
     <t>New Mobile Banking</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Note : 
+- Kolom isian tidak boleh kosong
+- Pastikan seluruh kolom yang kosong </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dihapus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, dengan cara blok kolom yang kosong kemudian klik kanan -&gt; pilih delete  -&gt; ok</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +106,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,11 +146,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,6 +176,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,21 +479,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270B27F8-6628-4531-966A-4408389C0925}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -449,8 +508,11 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -466,5 +528,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>